<commit_message>
manejo del sistema para tablas
se añadieron funciones para el manejo de informacion en vase a paginas que manejen tablas de informacion, por lo cual, la extraccion de datos por medio de una tabla o medio de selectores css esta totalmente funcional
</commit_message>
<xml_diff>
--- a/productos_amazon.xlsx
+++ b/productos_amazon.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="113">
   <si>
     <t>Producto</t>
   </si>
@@ -28,58 +28,64 @@
     <t>SAMSUNG Celular Galaxy A15 Negro 4GB RAM 128GB, Nacional con Garantía</t>
   </si>
   <si>
+    <t>Samsung Celular Galaxy M15 5G Gris 4GB RAM 128GB, Nacional con Garantía</t>
+  </si>
+  <si>
     <t>SAMSUNG Celular Galaxy A05 Plata 4GB RAM 64GB, Nacional con Garantía</t>
   </si>
   <si>
+    <t>Samsung Galaxy A15 Dual Sim 128GB Light Blue 6GB Ram Desbloqueado 6.5"</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A05S 4GB 128GB Violeta</t>
+  </si>
+  <si>
     <t>SAMSUNG Galaxy A05 4+128GB Negro</t>
   </si>
   <si>
     <t>Samsung Celular Galaxy A35 5G Azul Claro 6GB RAM 128GB, Nacional con Garantía</t>
   </si>
   <si>
-    <t>Samsung Galaxy A15 Dual Sim 128GB Light Blue 6GB Ram Desbloqueado 6.5"</t>
-  </si>
-  <si>
-    <t>SAMSUNG Celular Galaxy S23 FE Grafito 8GB RAM 256GB, AI, Nacional con Garantía</t>
-  </si>
-  <si>
-    <t>Samsung Celular Galaxy M15 5G Gris 4GB RAM 128GB, Nacional con Garantía</t>
+    <t>SAMSUNG Celular Galaxy S23 FE Morado 8GB RAM 128GB, AI, Nacional con Garantía</t>
+  </si>
+  <si>
+    <t>SAMSUNG Celular Galaxy M35 5G Azul Claro 6GB RAM 128GB, Nacional con Garantía</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Fit3 Grafito</t>
+  </si>
+  <si>
+    <t>Samsung Celular Galaxy M55 5G Verde 8GB RAM 128GB, Nacional con Garantía</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy S24 Ultra, Violeta, 12GB_256GB</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S23 Ultra 8GB_256GB Verde Desbloqueado</t>
   </si>
   <si>
     <t>SAMSUNG Galaxy A55 256gb 8GB Azul Oscuro</t>
   </si>
   <si>
-    <t>SAMSUNG Galaxy S24 Ultra, Violeta, 12GB_256GB</t>
-  </si>
-  <si>
     <t>SAMSUNG Galaxy A15 8+256GB Amarillo 5G</t>
   </si>
   <si>
     <t>SAMSUNG Celular Galaxy A25 5G Negro 6GB RAM 128GB, Nacional con Garantía</t>
   </si>
   <si>
-    <t>Samsung Galaxy Fit3 Grafito</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy S23 Ultra 8GB_256GB Verde Desbloqueado</t>
+    <t>SAMSUNG Galaxy A15 5G Azull Claro, 4GB_128GB</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A15 Dual Sim 128GB Blue Black 6GB Ram Desbloqueado 6.5"</t>
   </si>
   <si>
     <t>Samsung Galaxy S21 5G, versión estadounidense, 128 GB, Phantom Gray - desbloqueado (Reacondicionado)</t>
   </si>
   <si>
-    <t>Samsung Galaxy A15 Dual Sim 128GB Blue Black 6GB Ram Desbloqueado 6.5"</t>
-  </si>
-  <si>
-    <t>SAMSUNG Celular Galaxy M35 5G Azul Claro 6GB RAM 128GB, Nacional con Garantía</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy A05S 4GB 128GB Violeta</t>
-  </si>
-  <si>
-    <t>Samsung Celular Galaxy M55 5G Verde 8GB RAM 128GB, Nacional con Garantía</t>
-  </si>
-  <si>
-    <t>SAMSUNG Galaxy A15 5G Azull Claro, 4GB_128GB</t>
+    <t>Cables USB C cortos de 1 pie Fasgear 3A de carga rápida USB A a tipo C 2.0 cable de carga trenzado de sincronización de datos compatible con Galaxy S24/ i-Pad 2022/ estación de carga (4 colores)</t>
+  </si>
+  <si>
+    <t>UGREEN Funda para Galaxy S24 Transparente, Case Anti-Amarillo con Protección contra Caídas, Carcasa Samsung S24 Resistente a Arañazos y Roturas</t>
   </si>
   <si>
     <t>Fanmingsidi Funda para Samsung Galaxy A04 Carcasa con 360 Grados Metálico Anillo Hard PC Silicona Antigolpes Case para Samsung Galaxy A04 Negro</t>
@@ -88,172 +94,172 @@
     <t>X-Doria Revel Lux - Funda para iPhone X, Grado Militar, Prueba de caídas, Aluminio Coque para iPhone X, Color Negro Mate</t>
   </si>
   <si>
+    <t>SAMSUNG Galaxy A05S 4GB 128GB Negro</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S23 5G (128 GB, 8 GB) 6.1" AMOLED 2X, cámara 50MP, Global Volte, desbloqueado para todas las compañías (con cargador súper rápido de 25 W, Negro Phantom (Reacondicionado)</t>
+  </si>
+  <si>
+    <t>Samsung Pantalla QLED 4K de 55 Pulgadas (QN55Q65DAFXZX)</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy A35 8GB 256GB 5G Negro</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy A35 8GB 128GB 5G Negro</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy Tab S9 FE+ Menta 8GB RAM 128GB, Spen, Smart Book Cover, Nacional con Garantía</t>
+  </si>
+  <si>
+    <t>SAMSUNG Audifonos inalámbricos Galaxy Buds3 Grafito, AI, Nacional con Garantía</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy A55 8GB 128GB 5G Azul</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S22 256GB Bora Purple (Versión Nacional)</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A05s 4GB/128GB Verde (Light Green) Dual SIM SM-A057G</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Tab S9 Ultra Beige 12GB RAM 512GB, AI, Spen, Nacional con Garantía</t>
+  </si>
+  <si>
+    <t>SAMSUNG Celular Galaxy A25 5G 8GB 256GB 6.5" FHD+ 120 Hz 50 MP Blue Black</t>
+  </si>
+  <si>
+    <t>SAMSUNG R930 Galaxy Watch 6 BT 40 mm Modelo UE Graphite</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S21 5G desbloqueado de fábrica Versión US 5G 8K Video, 64MP High Res128GB, Phantom Violet (SM-G991UZVAXAA) (Reacondicionado)</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A25 5G Dual Sim 128GB Blue Black 6GB Ram Desbloqueado 6.5"</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S21+ 5G, versión estadounidense, 128GB, Phantom Black - desbloqueado (Reacondicionado)</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy A34 5G Negro</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy A54 256GB_5G Negro</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy A55 8Gb 128Gb 5g Negro</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy Tab A9+, 8GB RAM, 128GB, Color Gris Grafito</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S22 Ultra, 5G, desbloqueado de fábrica 128GB, SM-S908U1 (reacondicionado) (borgoña)</t>
+  </si>
+  <si>
+    <t>SAMSUNG Celular Galaxy M34 5G Azul obscuro 6GB RAM 128GB, Nacional con Garantía</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Tab S6 Lite 2024 Color Verde Claro RAM 4GB 128GB</t>
+  </si>
+  <si>
+    <t>SAMSUNG Pantalla 85" UHD 4K UN85CU70000FXZX</t>
+  </si>
+  <si>
+    <t>SAMSUNG Celular Galaxy S23 128GB Negro</t>
+  </si>
+  <si>
+    <t>Samsung Pantalla UHD de 65 Pulgadas (UN65DU8000FXZX)</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S21 5G, versión estadounidense, 128GB, Phantom Pink - desbloqueado (Reacondicionado)</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy Z Flip 4 SM-F721U1 - Desbloqueado de fábrica (256 GB, oro rosa)</t>
+  </si>
+  <si>
+    <t>Bigqin 5 Piezas Funda con Protector Pantalla Compatible con Samsung Galaxy Watch 7 40mm, PC Carcasa HD Cristal Templado Protector Ultra-Thin Anti-Rasguños, 5 Colores</t>
+  </si>
+  <si>
     <t>Protector de pantalla [2 Paq] para Samsung Galaxy S22 5G, RKINC película Mica de vidrio templado, compatible con huellas dactilares [Garantía de por vida] [Anti-rasguño] [Anti-rotura] [Sin burbujas]</t>
   </si>
   <si>
-    <t>Protector de pantalla [3 Paq] para Samsung Galaxy A53 5G/A52s 5G/A52 4G/5G / Oppo Reno 7 4G / Reno 8 5G, RKINC película de vidrio templado, 0.33 mm [Garantía de por vida] [Anti-rasguño][Sin burbujas]</t>
-  </si>
-  <si>
-    <t>SAMSUNG Audifonos inalámbricos Galaxy Buds3 Grafito, AI, Nacional con Garantía</t>
-  </si>
-  <si>
-    <t>SAMSUNG Galaxy A55 8GB 128GB 5G Azul</t>
-  </si>
-  <si>
-    <t>SAMSUNG Galaxy A35 8GB 256GB 5G Negro</t>
-  </si>
-  <si>
-    <t>Samsung Pantalla QLED 4K de 55 Pulgadas (QN55Q65DAFXZX)</t>
-  </si>
-  <si>
-    <t>SAMSUNG Galaxy A05S 4GB 128GB Negro</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy S21+ 5G, versión estadounidense, 128GB, Phantom Black - desbloqueado (Reacondicionado)</t>
-  </si>
-  <si>
-    <t>SAMSUNG Galaxy Tab A9+, 8GB RAM, 128GB, Color Gris Grafito</t>
-  </si>
-  <si>
-    <t>SAMSUNG Galaxy Tab S9 FE+ Menta 8GB RAM 128GB, Spen, Smart Book Cover, Nacional con Garantía</t>
-  </si>
-  <si>
-    <t>SAMSUNG Celular Galaxy A25 5G 8GB 256GB 6.5" FHD+ 120 Hz 50 MP Blue Black</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy Tab S6 Lite 2024 Color Verde Claro RAM 4GB 128GB</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy Tab S9 Ultra Beige 12GB RAM 512GB, AI, Spen, Nacional con Garantía</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy S22 256GB Bora Purple (Versión Nacional)</t>
-  </si>
-  <si>
-    <t>SAMSUNG R930 Galaxy Watch 6 BT 40 mm Modelo UE Graphite</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy A25 5G Dual Sim 128GB Blue Black 6GB Ram Desbloqueado 6.5"</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy S21 5G desbloqueado de fábrica Versión US 5G 8K Video, 64MP High Res128GB, Phantom Violet (SM-G991UZVAXAA) (Reacondicionado)</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy A05s 4GB/128GB Verde (Light Green) Dual SIM SM-A057G</t>
-  </si>
-  <si>
-    <t>SAMSUNG Galaxy A55 8Gb 128Gb 5g Negro</t>
-  </si>
-  <si>
-    <t>Samsung S22+ 128GB Verde desbloqueado (reacondicionado)</t>
-  </si>
-  <si>
-    <t>SAMSUNG Galaxy Z Flip 3 5G F711U AT&amp;T 128GB Lavanda (reacondicionado)</t>
-  </si>
-  <si>
-    <t>Samsung Pantalla UHD de 65 Pulgadas (UN65DU8000FXZX)</t>
-  </si>
-  <si>
-    <t>SAMSUNG Celular Galaxy S23 128GB Negro</t>
-  </si>
-  <si>
-    <t>SAMSUNG Galaxy A54 256GB_5G Negro</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy S22 Ultra, 5G, desbloqueado de fábrica 128GB, SM-S908U1 (reacondicionado) (borgoña)</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy A25 5G 6.5" FHD+ 256GB 8GB Blue</t>
-  </si>
-  <si>
-    <t>SAMSUNG Celular Galaxy M34 5G Azul obscuro 6GB RAM 128GB, Nacional con Garantía</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy S23 5G (128 GB, 8 GB) 6.1" AMOLED 2X, cámara 50MP, Global Volte, desbloqueado para todas las compañías (con cargador súper rápido de 25 W, Negro Phantom (Reacondicionado)</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy S21 5G, versión estadounidense, 128GB, Phantom Pink - desbloqueado (Reacondicionado)</t>
-  </si>
-  <si>
-    <t>SAMSUNG Galaxy A51 6GB 128GB Negro</t>
+    <t>Auslbin Funda para Tablet de PU Compatible con Samsung Galaxy Tab A9 Plus / A9+ 11" 2023, Funda de Cuero para Tab con Patrones geométricos para Tab A9 Plus SM-X210 /X215, Verde</t>
+  </si>
+  <si>
+    <t>YAPANIZCEL Funda para Samsung A14 5G, para Mujer con Brillantes COMPUESTA DE Tres Piezas Resistente (Transparente)</t>
   </si>
   <si>
     <t>3 Unidad Funda Impermeable para Celular, Funda Flotante para iPhone, Samsung Galaxy, Huawei, HTC, LG, Sony, Nokia, Motorola y MAS</t>
   </si>
   <si>
-    <t>Auslbin Funda para Tablet de PU Compatible con Samsung Galaxy Tab A9 Plus / A9+ 11" 2023, Funda de Cuero para Tab con Patrones geométricos para Tab A9 Plus SM-X210 /X215, Verde</t>
-  </si>
-  <si>
-    <t>Simpeak 2 Piezas Protector Pantalla Compatible con Samsung Galaxy Tab A9 Plus 11", Mica Tablet HD Cristal Película Templado Premium Complet Compatible con Galaxy Tab A9 Plus 2023 [No Bubble][Anti-Huella]</t>
-  </si>
-  <si>
-    <t>ZHIYIWU - Funda protectora de silicona para Samsung Galaxy A14 5G, a prueba de golpes, con soporte para anillo, soporte de anillo, duradera y suave TPU antiarañazos, no amarillenta</t>
-  </si>
-  <si>
-    <t>SAMSUNG DA29-00020B - Filtro de Agua (Color Blanco)</t>
-  </si>
-  <si>
-    <t>The Perfect Dust Cover LLC - Funda para Samsung Xpress SL-C430W (nailon, impermeable, antiestática), color azul marino</t>
+    <t>SAMSUNG, Pantalla QLED de 65" Class Q60 Series, QLED 4K Smart TV, Quantum Processor Lite, Q-Symphony 3.0, Ultimate UHD Dimming, QN65Q60CDFXZA</t>
   </si>
   <si>
     <t>KepaiTok Funda para Samsung Galaxy Tab A7 Lite de 8,7 Pulgadas 2021 (SM-T220/T225/T227), 2 en 1 Resistente a los Golpes, Funda Protectora para Galaxy Tab A7 Lite con Soporte (Negra)</t>
   </si>
   <si>
-    <t>Bateria DMW-BMB9E Camara Fotografica LUMIX, Compatible: DMC-FZ40, FZ100,FZ40K,FZ47, FZ47K, FZ100GK, FZ150K,FZ40GK,FZ45, FZ47GK,FZ48,FZ150GK,FZ70K,FZ45,FZ48,FZ100K,FZ150K,FZ100GK,FZ47GK,FZ60,FZ62,FZ72</t>
-  </si>
-  <si>
     <t>6,399</t>
   </si>
   <si>
-    <t>2,195</t>
+    <t>2,666</t>
+  </si>
+  <si>
+    <t>2,475</t>
+  </si>
+  <si>
+    <t>2,671</t>
+  </si>
+  <si>
+    <t>2,599</t>
   </si>
   <si>
     <t>1,895</t>
   </si>
   <si>
-    <t>5,110</t>
-  </si>
-  <si>
-    <t>2,699</t>
-  </si>
-  <si>
-    <t>9,389</t>
-  </si>
-  <si>
-    <t>3,249</t>
-  </si>
-  <si>
-    <t>6,708</t>
+    <t>3,779</t>
+  </si>
+  <si>
+    <t>10,330</t>
+  </si>
+  <si>
+    <t>3,699</t>
+  </si>
+  <si>
+    <t>745</t>
+  </si>
+  <si>
+    <t>5,499</t>
   </si>
   <si>
     <t>19,999</t>
   </si>
   <si>
+    <t>15,199</t>
+  </si>
+  <si>
+    <t>6,898</t>
+  </si>
+  <si>
     <t>3,298</t>
   </si>
   <si>
     <t>3,966</t>
   </si>
   <si>
-    <t>745</t>
-  </si>
-  <si>
-    <t>15,199</t>
-  </si>
-  <si>
-    <t>4,567</t>
-  </si>
-  <si>
-    <t>4,998</t>
-  </si>
-  <si>
-    <t>2,259</t>
-  </si>
-  <si>
-    <t>9,278</t>
-  </si>
-  <si>
-    <t>2,899</t>
+    <t>3,999</t>
+  </si>
+  <si>
+    <t>2,149</t>
+  </si>
+  <si>
+    <t>4,529</t>
+  </si>
+  <si>
+    <t>259</t>
+  </si>
+  <si>
+    <t>263</t>
   </si>
   <si>
     <t>199</t>
@@ -262,109 +268,91 @@
     <t>399</t>
   </si>
   <si>
+    <t>2,240</t>
+  </si>
+  <si>
+    <t>7,990</t>
+  </si>
+  <si>
+    <t>13,495</t>
+  </si>
+  <si>
+    <t>5,894</t>
+  </si>
+  <si>
+    <t>4,837</t>
+  </si>
+  <si>
+    <t>6,999</t>
+  </si>
+  <si>
+    <t>2,499</t>
+  </si>
+  <si>
+    <t>9,699</t>
+  </si>
+  <si>
+    <t>2,246</t>
+  </si>
+  <si>
+    <t>17,999</t>
+  </si>
+  <si>
+    <t>4,844</t>
+  </si>
+  <si>
+    <t>3,649</t>
+  </si>
+  <si>
+    <t>3,639</t>
+  </si>
+  <si>
+    <t>5,483</t>
+  </si>
+  <si>
+    <t>6,910</t>
+  </si>
+  <si>
+    <t>10,879</t>
+  </si>
+  <si>
+    <t>6,437</t>
+  </si>
+  <si>
+    <t>4,299</t>
+  </si>
+  <si>
+    <t>19,376</t>
+  </si>
+  <si>
+    <t>15,999</t>
+  </si>
+  <si>
+    <t>11,999</t>
+  </si>
+  <si>
+    <t>7,397</t>
+  </si>
+  <si>
+    <t>238</t>
+  </si>
+  <si>
     <t>159</t>
   </si>
   <si>
-    <t>149</t>
-  </si>
-  <si>
-    <t>2,499</t>
-  </si>
-  <si>
-    <t>6,324</t>
-  </si>
-  <si>
-    <t>5,894</t>
-  </si>
-  <si>
-    <t>13,495</t>
-  </si>
-  <si>
-    <t>2,240</t>
-  </si>
-  <si>
-    <t>4,992</t>
-  </si>
-  <si>
-    <t>3,898</t>
-  </si>
-  <si>
-    <t>6,999</t>
-  </si>
-  <si>
-    <t>4,844</t>
-  </si>
-  <si>
-    <t>4,299</t>
-  </si>
-  <si>
-    <t>17,999</t>
-  </si>
-  <si>
-    <t>9,699</t>
-  </si>
-  <si>
-    <t>3,649</t>
-  </si>
-  <si>
-    <t>3,644</t>
-  </si>
-  <si>
-    <t>4,515</t>
-  </si>
-  <si>
-    <t>2,246</t>
-  </si>
-  <si>
-    <t>7,510</t>
-  </si>
-  <si>
-    <t>5,347</t>
-  </si>
-  <si>
-    <t>11,999</t>
-  </si>
-  <si>
-    <t>11,799</t>
-  </si>
-  <si>
-    <t>6,910</t>
-  </si>
-  <si>
-    <t>10,421</t>
-  </si>
-  <si>
-    <t>6,437</t>
-  </si>
-  <si>
-    <t>7,990</t>
-  </si>
-  <si>
-    <t>4,415</t>
+    <t>309</t>
+  </si>
+  <si>
+    <t>194</t>
   </si>
   <si>
     <t>189</t>
   </si>
   <si>
-    <t>309</t>
-  </si>
-  <si>
-    <t>209</t>
-  </si>
-  <si>
-    <t>330</t>
-  </si>
-  <si>
-    <t>599</t>
-  </si>
-  <si>
-    <t>473</t>
+    <t>14,999</t>
   </si>
   <si>
     <t>299</t>
-  </si>
-  <si>
-    <t>540</t>
   </si>
 </sst>
 </file>
@@ -741,7 +729,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -749,28 +737,28 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -778,7 +766,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -786,7 +774,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -794,7 +782,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -802,7 +790,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -810,7 +798,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -818,7 +806,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -826,7 +814,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -834,7 +822,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -842,7 +830,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -850,13 +838,16 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
@@ -982,16 +973,13 @@
       <c r="A33" t="s">
         <v>33</v>
       </c>
-      <c r="B33" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -999,7 +987,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1007,7 +995,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1015,7 +1003,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1023,7 +1011,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1031,7 +1019,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1039,7 +1027,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1047,7 +1035,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1060,31 +1048,25 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
-      <c r="B44" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
-      <c r="B45" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1092,7 +1074,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1100,20 +1082,23 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
+      <c r="B49" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1121,7 +1106,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1129,20 +1114,23 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>53</v>
       </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1150,7 +1138,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1158,7 +1146,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1166,7 +1154,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1174,7 +1162,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1182,23 +1170,23 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>